<commit_message>
absolute to relative path rest 1-6 cases
</commit_message>
<xml_diff>
--- a/Resources/log_in_credentials.xlsx
+++ b/Resources/log_in_credentials.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">superadmin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d7QUVg</t>
   </si>
 </sst>
 </file>
@@ -136,7 +133,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -156,8 +153,8 @@
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+      <c r="B2" s="1" t="n">
+        <v>12345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>